<commit_message>
New name for recuperation magic better fits in with what it does
</commit_message>
<xml_diff>
--- a/CoreRulebook/Data/Archetypes/Auror.xlsx
+++ b/CoreRulebook/Data/Archetypes/Auror.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t xml:space="preserve">LVL</t>
   </si>
@@ -43,16 +43,13 @@
     <t xml:space="preserve">Spellcasting Improvement</t>
   </si>
   <si>
+    <t xml:space="preserve">Sudden Ambush</t>
+  </si>
+  <si>
     <t xml:space="preserve">Multiward</t>
   </si>
   <si>
-    <t xml:space="preserve">Shocking Arrival</t>
-  </si>
-  <si>
     <t xml:space="preserve">Defence Against the Dark Arts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ambush</t>
   </si>
   <si>
     <t xml:space="preserve">Terrain Advantage</t>
@@ -174,12 +171,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -192,14 +189,15 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="41.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="41.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.88"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -243,9 +241,6 @@
       <c r="C3" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -256,6 +251,9 @@
         <v>0</v>
       </c>
       <c r="D4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>8</v>
       </c>
     </row>
@@ -270,11 +268,8 @@
       <c r="C5" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="E5" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -295,10 +290,10 @@
         <v>1</v>
       </c>
       <c r="C7" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>12</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -313,7 +308,7 @@
         <v>6</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -325,7 +320,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -337,7 +332,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -349,7 +344,7 @@
         <v>2</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -361,7 +356,7 @@
         <v>2</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -376,7 +371,7 @@
         <v>6</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -388,7 +383,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -409,10 +404,10 @@
         <v>3</v>
       </c>
       <c r="C16" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="0" t="s">
         <v>21</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Actions and resist revamps
</commit_message>
<xml_diff>
--- a/CoreRulebook/Data/Archetypes/Auror.xlsx
+++ b/CoreRulebook/Data/Archetypes/Auror.xlsx
@@ -88,7 +88,7 @@
     <t xml:space="preserve">Magic Cleave</t>
   </si>
   <si>
-    <t xml:space="preserve">Combat Reflexes</t>
+    <t xml:space="preserve">Merciless Strike (use 1 bigger dice on damage checks)</t>
   </si>
   <si>
     <t xml:space="preserve">Incredible Resilience (see: hard to kill)</t>
@@ -197,8 +197,8 @@
   </sheetPr>
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32:C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>